<commit_message>
Gráficas de número de bicicletas por hora en cada una de las estaciones
</commit_message>
<xml_diff>
--- a/Datos en excel.xlsx
+++ b/Datos en excel.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmedi\OneDrive\Escritorio\modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98FC86D-53F2-4F49-9E16-22C2CD9EB848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1637C59-C9D8-44CA-92CF-2B843A828865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{C5858227-68FA-4971-A13C-0E196BDB9152}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C5858227-68FA-4971-A13C-0E196BDB9152}"/>
   </bookViews>
   <sheets>
     <sheet name="DATOS" sheetId="1" r:id="rId1"/>
     <sheet name="Modelo Gaussiano" sheetId="2" r:id="rId2"/>
     <sheet name="HORAS PICO EN ESTACIONES" sheetId="3" r:id="rId3"/>
+    <sheet name="Matrices de probabilidad" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="62">
   <si>
     <t>Estación</t>
   </si>
@@ -172,9 +173,6 @@
     <t>Valor en distribucion</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>Tendencias observadas:</t>
   </si>
   <si>
@@ -279,12 +277,34 @@
   <si>
     <t>Peso fuerte a las 6:45 → llegada temprana a Uriel.</t>
   </si>
+  <si>
+    <t>origen/
+destino</t>
+  </si>
+  <si>
+    <t>Matriz de probabilidades jornada de la mañana</t>
+  </si>
+  <si>
+    <t>Matriz de probabilidades jornada de la media tarde</t>
+  </si>
+  <si>
+    <t>Matriz de probabilidades jornada de la tarde</t>
+  </si>
+  <si>
+    <t>6 9</t>
+  </si>
+  <si>
+    <t>9 13</t>
+  </si>
+  <si>
+    <t>13 16</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,6 +314,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -454,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -467,35 +495,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -508,7 +540,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -521,12 +553,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5600,7 +5637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E68A239-ACC5-4254-B21C-D8A90D40B18A}">
   <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="94" workbookViewId="0">
+    <sheetView zoomScale="94" workbookViewId="0">
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
@@ -5888,10 +5925,10 @@
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="9" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -5914,10 +5951,10 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="8">
         <v>18763</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -5926,24 +5963,24 @@
       <c r="E13" s="3">
         <v>4109</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="18">
         <v>2785</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13" s="18">
         <v>903</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="18">
         <v>5672</v>
       </c>
-      <c r="I13" s="16">
+      <c r="I13" s="18">
         <v>5294</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="8">
         <v>27791</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -5952,24 +5989,24 @@
       <c r="E14" s="3">
         <v>6062</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="18">
         <v>3886</v>
       </c>
-      <c r="G14" s="16">
+      <c r="G14" s="18">
         <v>1339</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="18">
         <v>8836</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="18">
         <v>7668</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="8">
         <v>29174</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -5978,24 +6015,24 @@
       <c r="E15" s="3">
         <v>6135</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="18">
         <v>4144</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="18">
         <v>1453</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="18">
         <v>9296</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I15" s="18">
         <v>8146</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="8">
         <v>26000</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -6004,24 +6041,24 @@
       <c r="E16" s="3">
         <v>5690</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="18">
         <v>3509</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G16" s="18">
         <v>1249</v>
       </c>
-      <c r="H16" s="16">
+      <c r="H16" s="18">
         <v>8674</v>
       </c>
-      <c r="I16" s="16">
+      <c r="I16" s="18">
         <v>6878</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="8">
         <v>25345</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -6030,24 +6067,24 @@
       <c r="E17" s="3">
         <v>5759</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="18">
         <v>3886</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G17" s="18">
         <v>1381</v>
       </c>
-      <c r="H17" s="16">
+      <c r="H17" s="18">
         <v>7847</v>
       </c>
-      <c r="I17" s="16">
+      <c r="I17" s="18">
         <v>6472</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="8">
         <f>SUM(B13:B17)</f>
         <v>127073</v>
       </c>
@@ -6076,15 +6113,15 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G22" s="17" t="s">
+      <c r="G22" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G23" s="2" t="s">
@@ -6266,149 +6303,149 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="G30" s="20" t="s">
+      <c r="G30" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="H30" s="20">
+      <c r="H30" s="22">
         <f>SUM(H25:H29)</f>
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="9"/>
-      <c r="B43" s="10"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="12"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="11"/>
-      <c r="B44" s="12"/>
+      <c r="A44" s="13"/>
+      <c r="B44" s="14"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="11"/>
-      <c r="B45" s="12"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="14"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="11"/>
-      <c r="B46" s="12"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="14"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="11"/>
-      <c r="B47" s="12"/>
+      <c r="A47" s="13"/>
+      <c r="B47" s="14"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="11"/>
-      <c r="B48" s="12"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="14"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="9"/>
-      <c r="B49" s="10"/>
+      <c r="A49" s="11"/>
+      <c r="B49" s="12"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="11"/>
-      <c r="B50" s="12"/>
+      <c r="A50" s="13"/>
+      <c r="B50" s="14"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="11"/>
-      <c r="B51" s="12"/>
+      <c r="A51" s="13"/>
+      <c r="B51" s="14"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="11"/>
-      <c r="B52" s="12"/>
+      <c r="A52" s="13"/>
+      <c r="B52" s="14"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="11"/>
-      <c r="B53" s="12"/>
+      <c r="A53" s="13"/>
+      <c r="B53" s="14"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="11"/>
-      <c r="B54" s="12"/>
+      <c r="A54" s="13"/>
+      <c r="B54" s="14"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="9"/>
-      <c r="B55" s="10"/>
+      <c r="A55" s="11"/>
+      <c r="B55" s="12"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="11"/>
-      <c r="B56" s="12"/>
+      <c r="A56" s="13"/>
+      <c r="B56" s="14"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="11"/>
-      <c r="B57" s="12"/>
+      <c r="A57" s="13"/>
+      <c r="B57" s="14"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="11"/>
-      <c r="B58" s="12"/>
+      <c r="A58" s="13"/>
+      <c r="B58" s="14"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="11"/>
-      <c r="B59" s="12"/>
+      <c r="A59" s="13"/>
+      <c r="B59" s="14"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="11"/>
-      <c r="B60" s="12"/>
+      <c r="A60" s="13"/>
+      <c r="B60" s="14"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="9"/>
-      <c r="B61" s="10"/>
+      <c r="A61" s="11"/>
+      <c r="B61" s="12"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="11"/>
-      <c r="B62" s="12"/>
+      <c r="A62" s="13"/>
+      <c r="B62" s="14"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="11"/>
-      <c r="B63" s="12"/>
+      <c r="A63" s="13"/>
+      <c r="B63" s="14"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="11"/>
-      <c r="B64" s="12"/>
+      <c r="A64" s="13"/>
+      <c r="B64" s="14"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="11"/>
-      <c r="B65" s="12"/>
+      <c r="A65" s="13"/>
+      <c r="B65" s="14"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="11"/>
-      <c r="B66" s="12"/>
+      <c r="A66" s="13"/>
+      <c r="B66" s="14"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="9"/>
-      <c r="B67" s="10"/>
+      <c r="A67" s="11"/>
+      <c r="B67" s="12"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="11"/>
-      <c r="B68" s="12"/>
+      <c r="A68" s="13"/>
+      <c r="B68" s="14"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="11"/>
-      <c r="B69" s="12"/>
+      <c r="A69" s="13"/>
+      <c r="B69" s="14"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="11"/>
-      <c r="B70" s="12"/>
+      <c r="A70" s="13"/>
+      <c r="B70" s="14"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="11"/>
-      <c r="B71" s="12"/>
+      <c r="A71" s="13"/>
+      <c r="B71" s="14"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="11"/>
-      <c r="B72" s="12"/>
+      <c r="A72" s="13"/>
+      <c r="B72" s="14"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="9"/>
-      <c r="B73" s="9"/>
+      <c r="A73" s="11"/>
+      <c r="B73" s="11"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="11"/>
-      <c r="B74" s="13"/>
+      <c r="A74" s="13"/>
+      <c r="B74" s="15"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="14"/>
-      <c r="B75" s="15"/>
+      <c r="A75" s="16"/>
+      <c r="B75" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -6430,10 +6467,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{163E83C8-0AD2-490A-BA44-4D2BA775B24A}">
-  <dimension ref="A1:K401"/>
+  <dimension ref="A1:J401"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6441,7 +6478,7 @@
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>34</v>
       </c>
@@ -6452,7 +6489,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>6.75</v>
       </c>
@@ -6463,7 +6500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>9</v>
       </c>
@@ -6478,11 +6515,8 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>11</v>
       </c>
@@ -6498,7 +6532,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>13</v>
       </c>
@@ -6514,7 +6548,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>14</v>
       </c>
@@ -6530,7 +6564,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>16</v>
       </c>
@@ -6541,7 +6575,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -6549,7 +6583,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6.3</v>
       </c>
@@ -6558,7 +6592,7 @@
         <v>7.9559508718227576E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>A11+0.025</f>
         <v>6.3250000000000002</v>
@@ -6568,7 +6602,7 @@
         <v>0.10457900128900169</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" ref="A13:A76" si="0">A12+0.025</f>
         <v>6.3500000000000005</v>
@@ -6578,7 +6612,7 @@
         <v>0.13533528323661345</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>6.3750000000000009</v>
@@ -6587,9 +6621,9 @@
         <f t="shared" si="1"/>
         <v>0.17242162389375434</v>
       </c>
-      <c r="G14" s="21"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G14" s="23"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>6.4000000000000012</v>
@@ -6598,9 +6632,9 @@
         <f t="shared" si="1"/>
         <v>0.21626516682988978</v>
       </c>
-      <c r="G15" s="21"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G15" s="23"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>6.4250000000000016</v>
@@ -10473,8 +10507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E5BA67-D1A1-4817-927D-6D502C123DDF}">
   <dimension ref="B2:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6:N36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10485,11 +10519,11 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
       <c r="J2" s="2" t="s">
         <v>3</v>
       </c>
@@ -10611,7 +10645,7 @@
       <c r="L6" s="3">
         <v>0.4</v>
       </c>
-      <c r="N6" s="26" t="s">
+      <c r="N6" s="28" t="s">
         <v>5</v>
       </c>
     </row>
@@ -10645,9 +10679,9 @@
       <c r="D8" s="3">
         <v>0.5</v>
       </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
       <c r="J8" s="3">
         <v>16</v>
       </c>
@@ -10658,30 +10692,30 @@
         <v>0.3</v>
       </c>
       <c r="N8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="N9" s="29"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N10" s="29" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="N9" s="27"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="N10" s="27" t="s">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N11" s="29"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N12" s="29" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="N11" s="27"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="N12" s="27" t="s">
-        <v>46</v>
-      </c>
-    </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="N13" s="27"/>
+      <c r="N13" s="29"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
@@ -10694,11 +10728,11 @@
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="N14" s="27" t="s">
-        <v>47</v>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="N14" s="29" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="2:14" ht="43.2" x14ac:dyDescent="0.3">
@@ -10720,9 +10754,9 @@
       <c r="H15" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J15" s="22"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
     </row>
     <row r="16" spans="2:14" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
@@ -10743,10 +10777,10 @@
       <c r="H16" s="3">
         <v>0.7</v>
       </c>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="N16" s="26" t="s">
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="N16" s="28" t="s">
         <v>4</v>
       </c>
     </row>
@@ -10769,10 +10803,10 @@
       <c r="H17" s="3">
         <v>0.6</v>
       </c>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="N17" s="27"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="N17" s="29"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
@@ -10793,11 +10827,11 @@
       <c r="H18" s="3">
         <v>0.5</v>
       </c>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="N18" s="27" t="s">
-        <v>48</v>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="N18" s="29" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
@@ -10819,10 +10853,10 @@
       <c r="H19" s="3">
         <v>0.4</v>
       </c>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="N19" s="27"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="N19" s="29"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
@@ -10843,82 +10877,82 @@
       <c r="H20" s="3">
         <v>0.6</v>
       </c>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="N20" s="27" t="s">
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="N20" s="29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="N21" s="29"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="N22" s="29" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="N21" s="27"/>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="N22" s="27" t="s">
+    <row r="24" spans="2:14" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="N24" s="28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N25" s="29"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N26" s="29" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="2:14" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="N24" s="26" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="N25" s="27"/>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="N26" s="27" t="s">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N27" s="29"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N28" s="29" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="N27" s="27"/>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="N28" s="27" t="s">
+    <row r="30" spans="2:14" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="N30" s="28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N31" s="29"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N32" s="29" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="2:14" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="N30" s="26" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="N31" s="27"/>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="N32" s="27" t="s">
+    <row r="33" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N33" s="29"/>
+    </row>
+    <row r="34" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N34" s="29" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N33" s="27"/>
-    </row>
-    <row r="34" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N34" s="27" t="s">
+    <row r="35" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N35" s="29"/>
+    </row>
+    <row r="36" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N36" s="29" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N35" s="27"/>
-    </row>
-    <row r="36" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N36" s="27" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -10932,4 +10966,487 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92D2FA7E-B8BE-41E6-A921-1F8D314461BD}">
+  <dimension ref="B1:H27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="H3">
+        <f>SUM(C3:G3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H7" si="0">SUM(C4:G4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="H13">
+        <f>SUM(C13:G13)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.46</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ref="H14:H17" si="1">SUM(C14:G14)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.41</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.27</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B22" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.22</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0.35</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="G23" s="6">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H23">
+        <f>SUM(C23:G23)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0</v>
+      </c>
+      <c r="E24" s="6">
+        <v>0.35</v>
+      </c>
+      <c r="F24" s="6">
+        <v>0.42</v>
+      </c>
+      <c r="G24" s="6">
+        <v>0.11</v>
+      </c>
+      <c r="H24">
+        <f t="shared" ref="H24:H27" si="2">SUM(C24:G24)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0</v>
+      </c>
+      <c r="F25" s="6">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G25" s="6">
+        <v>0.32</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="E26" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="F26" s="6">
+        <v>0</v>
+      </c>
+      <c r="G26" s="6">
+        <v>0.53</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0.45</v>
+      </c>
+      <c r="D27" s="6">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0.32</v>
+      </c>
+      <c r="F27" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G27" s="6">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B21:G21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="H11" twoDigitTextYear="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>